<commit_message>
Update 22 Nov 5pm
</commit_message>
<xml_diff>
--- a/Models.xlsx
+++ b/Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harnham-my.sharepoint.com/personal/annalisasmith_rockborne_com/Documents/Documents/ML Project Oct-Nov 23/ML_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFEEEA4A-539A-43BF-8AD9-D0427CE9C915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{DFEEEA4A-539A-43BF-8AD9-D0427CE9C915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{390B7AA1-CBED-430D-AF1D-04C8DDD3404F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1CD2112-EFD6-47FA-84D1-DEBFC5C329C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D1CD2112-EFD6-47FA-84D1-DEBFC5C329C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Models</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>LogisticRegressor</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 score</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>0.98, 0.00, 0.18</t>
+  </si>
+  <si>
+    <t>0.86, 0.00,0.53</t>
+  </si>
+  <si>
+    <t>0.92, 0.00, 0.27</t>
+  </si>
+  <si>
+    <t>AUC - 1 vs rest</t>
+  </si>
+  <si>
+    <t>0.82, 0.71, 0.82</t>
+  </si>
+  <si>
+    <t>OverSampler</t>
+  </si>
+  <si>
+    <t>penalty='none',solver='lbfgs',max_iter=5000</t>
+  </si>
+  <si>
+    <t>0.66, 0.32, 0.59</t>
+  </si>
+  <si>
+    <t>0.59, 0.43, 0.51</t>
+  </si>
+  <si>
+    <t>0.63, 0.37, 0.54</t>
+  </si>
+  <si>
+    <t>0.79, 0.62, 0.72</t>
+  </si>
+  <si>
+    <t>UnderSampler</t>
+  </si>
+  <si>
+    <t>0.65, 0.29, 0.63</t>
+  </si>
+  <si>
+    <t>0.59, 0.42, 0.52</t>
+  </si>
+  <si>
+    <t>0.62, 0.34, 0.57</t>
+  </si>
+  <si>
+    <t>0.79, 0.60, 0.74</t>
+  </si>
+  <si>
+    <t>SMOTE</t>
+  </si>
+  <si>
+    <t>0.66, 0.34, 0.61</t>
+  </si>
+  <si>
+    <t>0.61, 0.45, 0.52</t>
+  </si>
+  <si>
+    <t>0.63, 0.38, 0.56</t>
+  </si>
+  <si>
+    <t>0.80, 0.64, 0.74</t>
+  </si>
+  <si>
+    <t>penalty='l2',solver='sag',max_iter=5000,C=1</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>dual=False</t>
+  </si>
+  <si>
+    <t>0.70, 0.24, 0.64</t>
+  </si>
+  <si>
+    <t>0.58, 0.45, 0.50</t>
+  </si>
+  <si>
+    <t>0.63, 0.31, 0.56</t>
+  </si>
+  <si>
+    <t>0.80, 0.61, 0.74</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>0.85, 0.93, 0.81</t>
+  </si>
+  <si>
+    <t>0.87, 0.90, 0.82</t>
+  </si>
+  <si>
+    <t>0.86, 0.92, 0.81</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>0.95, 0.97, 0.87</t>
+  </si>
+  <si>
+    <t>0.88, 0.98, 094</t>
+  </si>
+  <si>
+    <t>0.91, 0.97, 0.90</t>
+  </si>
+  <si>
+    <t>0.98, 0.99, 0.97</t>
+  </si>
+  <si>
+    <t>0.90, 0.94, 0.86</t>
+  </si>
+  <si>
+    <t>criterion='entropy',max_depth=None, min_samples_leaf=2, min_samples_split=2</t>
+  </si>
+  <si>
+    <t>0.90, 0.94, 0.78</t>
+  </si>
+  <si>
+    <t>0.85, 0.90, 0.86</t>
+  </si>
+  <si>
+    <t>0.88, 0.92, 081</t>
+  </si>
+  <si>
+    <t>0.93, 0.95, 0.88</t>
   </si>
 </sst>
 </file>
@@ -74,8 +230,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,20 +555,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1A2260-06E7-465F-8B09-FB5F7CB3A5C5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="68.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>